<commit_message>
HTA report submitted version. With EVPPI
</commit_message>
<xml_diff>
--- a/data/NHL_rate.xlsx
+++ b/data/NHL_rate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4898e5cc837f6cd5/Documents/Bristol/Coeliac review HTA/Coeliac_screening/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:40009_{16E6B02D-53F4-4CC6-AD7B-3ACB83598521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F5569D84-5B63-4020-9439-BBCCB412B0CF}"/>
+  <xr:revisionPtr revIDLastSave="44" documentId="13_ncr:40009_{16E6B02D-53F4-4CC6-AD7B-3ACB83598521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{65F5F1AC-4F1E-40BF-985C-D16F33EA0FBF}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mixed" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="33">
   <si>
     <t>Age group</t>
   </si>
@@ -126,13 +126,19 @@
   </si>
   <si>
     <t>0.34 (0.29-0.40)</t>
+  </si>
+  <si>
+    <t>0.03 (0.01-0.06)</t>
+  </si>
+  <si>
+    <t>0.38 (0.34-0.42)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -274,6 +280,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -456,7 +469,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -571,6 +584,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -616,11 +657,20 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -977,305 +1027,325 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y4"/>
+  <dimension ref="A1:Z5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="A1:Y3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="6" max="6" width="13.7890625" customWidth="1"/>
-    <col min="7" max="7" width="12.62890625" customWidth="1"/>
-    <col min="8" max="8" width="11.578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.3671875" customWidth="1"/>
-    <col min="10" max="10" width="15.68359375" customWidth="1"/>
-    <col min="11" max="11" width="11.578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.578125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.05078125" customWidth="1"/>
+    <col min="7" max="7" width="13.7890625" customWidth="1"/>
+    <col min="8" max="8" width="12.62890625" customWidth="1"/>
+    <col min="9" max="9" width="11.578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.3671875" customWidth="1"/>
+    <col min="11" max="11" width="15.68359375" customWidth="1"/>
+    <col min="12" max="12" width="11.578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:26" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>13</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:26" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A2" t="s">
         <v>24</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2">
+        <f>VALUE(LEFT(B2, FIND("(", B2) - 1))</f>
         <v>0.03</v>
       </c>
-      <c r="C2">
+      <c r="D2">
+        <f>VALUE(SUBSTITUTE(RIGHT(B2, LEN(B2) - FIND("(", B2)), _xlfn.CONCAT("-", SUBSTITUTE(RIGHT(B2, LEN(B2) - FIND("-", B2)), ")", ""), ")"), ""))</f>
         <v>0.01</v>
       </c>
-      <c r="D2">
+      <c r="E2">
+        <f>VALUE(SUBSTITUTE(RIGHT(B2, LEN(B2) - FIND("-", B2)), ")", ""))</f>
         <v>0.06</v>
       </c>
-      <c r="E2">
-        <f>B2/1000</f>
+      <c r="F2">
+        <f>C2/1000</f>
         <v>2.9999999999999997E-5</v>
       </c>
-      <c r="F2">
-        <f t="shared" ref="F2:G2" si="0">C2/1000</f>
+      <c r="G2">
+        <f t="shared" ref="G2:H2" si="0">D2/1000</f>
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <f t="shared" si="0"/>
         <v>5.9999999999999995E-5</v>
       </c>
-      <c r="H2">
-        <f>E2*3.28</f>
+      <c r="I2">
+        <f>F2*3.28</f>
         <v>9.8399999999999979E-5</v>
       </c>
-      <c r="I2">
+      <c r="J2">
+        <f>H2*3.28</f>
+        <v>1.9679999999999996E-4</v>
+      </c>
+      <c r="K2">
         <f>G2*3.28</f>
-        <v>1.9679999999999996E-4</v>
-      </c>
-      <c r="J2">
-        <f>F2*3.28</f>
         <v>3.2799999999999998E-5</v>
       </c>
-      <c r="K2">
-        <f>1-EXP(-H2)</f>
+      <c r="L2">
+        <f>1-EXP(-I2)</f>
         <v>9.8395158878772371E-5</v>
       </c>
-      <c r="L2">
-        <f t="shared" ref="L2:M3" si="1">1-EXP(-I2)</f>
+      <c r="M2">
+        <f t="shared" ref="M2:N3" si="1">1-EXP(-J2)</f>
         <v>1.967806361502511E-4</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <f t="shared" si="1"/>
         <v>3.2799462085897346E-5</v>
       </c>
-      <c r="N2">
-        <f>(L2-M2)/(2*1.96)</f>
+      <c r="O2">
+        <f>(M2-N2)/(2*1.96)</f>
         <v>4.1831932159273916E-5</v>
       </c>
-      <c r="O2" s="1">
-        <f t="shared" ref="O2:O3" si="2">(((1-K2)/(N2*N2))-(1/K2))*K2*K2</f>
+      <c r="P2" s="1">
+        <f t="shared" ref="P2:P3" si="2">(((1-L2)/(O2*O2))-(1/L2))*L2*L2</f>
         <v>5.5319870463342369</v>
       </c>
-      <c r="P2" s="1">
-        <f>O2*((1/K2)-1)</f>
+      <c r="Q2" s="1">
+        <f>P2*((1/L2)-1)</f>
         <v>56216.614604026443</v>
       </c>
-      <c r="Q2">
-        <f>E2*4.7</f>
+      <c r="R2">
+        <f>F2*4.7</f>
         <v>1.4099999999999998E-4</v>
       </c>
-      <c r="R2">
+      <c r="S2">
+        <f>H2*4.7</f>
+        <v>2.8199999999999997E-4</v>
+      </c>
+      <c r="T2">
         <f>G2*4.7</f>
-        <v>2.8199999999999997E-4</v>
-      </c>
-      <c r="S2">
-        <f>F2*4.7</f>
         <v>4.7000000000000004E-5</v>
       </c>
-      <c r="T2">
-        <f>1-EXP(-Q2)</f>
+      <c r="U2">
+        <f>1-EXP(-R2)</f>
         <v>1.4099005996714986E-4</v>
       </c>
-      <c r="U2">
-        <f t="shared" ref="U2:V3" si="3">1-EXP(-R2)</f>
+      <c r="V2">
+        <f t="shared" ref="V2:W3" si="3">1-EXP(-S2)</f>
         <v>2.8196024173732237E-4</v>
       </c>
-      <c r="V2">
+      <c r="W2">
         <f t="shared" si="3"/>
         <v>4.699889551729175E-5</v>
       </c>
-      <c r="W2">
-        <f>(U2-V2)/(2*1.96)</f>
+      <c r="X2">
+        <f>(V2-W2)/(2*1.96)</f>
         <v>5.993911893368128E-5</v>
       </c>
-      <c r="X2" s="1">
-        <f t="shared" ref="X2" si="4">(((1-T2)/(W2*W2))-(1/T2))*T2*T2</f>
+      <c r="Y2" s="1">
+        <f t="shared" ref="Y2" si="4">(((1-U2)/(X2*X2))-(1/U2))*U2*U2</f>
         <v>5.5320229992425576</v>
       </c>
-      <c r="Y2" s="1">
-        <f t="shared" ref="Y2" si="5">X2*((1/T2)-1)</f>
+      <c r="Z2" s="1">
+        <f t="shared" ref="Z2" si="5">Y2*((1/U2)-1)</f>
         <v>39231.439721898925</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:26" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A3" t="s">
         <v>25</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3">
+        <f>VALUE(LEFT(B3, FIND("(", B3) - 1))</f>
         <v>0.38</v>
       </c>
-      <c r="C3">
+      <c r="D3">
+        <f>VALUE(SUBSTITUTE(RIGHT(B3, LEN(B3) - FIND("(", B3)), _xlfn.CONCAT("-", SUBSTITUTE(RIGHT(B3, LEN(B3) - FIND("-", B3)), ")", ""), ")"), ""))</f>
         <v>0.34</v>
       </c>
-      <c r="D3">
+      <c r="E3" s="5" t="str">
+        <f>SUBSTITUTE(RIGHT(B3, LEN(B3) - FIND("-", B3)), ")", "")</f>
         <v>0.42</v>
       </c>
-      <c r="E3">
-        <f>B3/1000</f>
+      <c r="F3">
+        <f>C3/1000</f>
         <v>3.8000000000000002E-4</v>
       </c>
-      <c r="F3">
-        <f t="shared" ref="F3" si="6">C3/1000</f>
+      <c r="G3">
+        <f t="shared" ref="G3" si="6">D3/1000</f>
         <v>3.4000000000000002E-4</v>
       </c>
-      <c r="G3">
-        <f t="shared" ref="G3" si="7">D3/1000</f>
+      <c r="H3">
+        <f t="shared" ref="H3" si="7">E3/1000</f>
         <v>4.1999999999999996E-4</v>
       </c>
-      <c r="H3">
-        <f>E3*3.28</f>
+      <c r="I3">
+        <f>F3*3.28</f>
         <v>1.2463999999999999E-3</v>
       </c>
-      <c r="I3">
+      <c r="J3">
+        <f>H3*3.28</f>
+        <v>1.3775999999999999E-3</v>
+      </c>
+      <c r="K3">
         <f>G3*3.28</f>
-        <v>1.3775999999999999E-3</v>
-      </c>
-      <c r="J3">
-        <f>F3*3.28</f>
         <v>1.1152E-3</v>
       </c>
-      <c r="K3">
-        <f>1-EXP(-H3)</f>
+      <c r="L3">
+        <f>1-EXP(-I3)</f>
         <v>1.2456235661358894E-3</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <f t="shared" si="1"/>
         <v>1.37665154470068E-3</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <f t="shared" si="1"/>
         <v>1.1145783955726074E-3</v>
       </c>
-      <c r="N3">
-        <f>(L3-M3)/(2*1.96)</f>
+      <c r="O3">
+        <f>(M3-N3)/(2*1.96)</f>
         <v>6.6855395185732794E-5</v>
       </c>
-      <c r="O3" s="1">
+      <c r="P3" s="1">
         <f t="shared" si="2"/>
         <v>346.70319727135484</v>
       </c>
-      <c r="P3" s="1">
-        <f t="shared" ref="P3" si="8">O3*((1/K3)-1)</f>
+      <c r="Q3" s="1">
+        <f t="shared" ref="Q3" si="8">P3*((1/L3)-1)</f>
         <v>277990.3535966042</v>
       </c>
-      <c r="Q3">
-        <f>E3*4.7</f>
+      <c r="R3">
+        <f>F3*4.7</f>
         <v>1.7860000000000003E-3</v>
       </c>
-      <c r="R3">
+      <c r="S3">
+        <f>H3*4.7</f>
+        <v>1.9740000000000001E-3</v>
+      </c>
+      <c r="T3">
         <f>G3*4.7</f>
-        <v>1.9740000000000001E-3</v>
-      </c>
-      <c r="S3">
-        <f>F3*4.7</f>
         <v>1.5980000000000002E-3</v>
       </c>
-      <c r="T3">
-        <f>1-EXP(-Q3)</f>
+      <c r="U3">
+        <f>1-EXP(-R3)</f>
         <v>1.7844060510721071E-3</v>
       </c>
-      <c r="U3">
+      <c r="V3">
         <f t="shared" si="3"/>
         <v>1.972052943373992E-3</v>
       </c>
-      <c r="V3">
+      <c r="W3">
         <f t="shared" si="3"/>
         <v>1.5967238778382686E-3</v>
       </c>
-      <c r="W3">
-        <f>(U3-V3)/(2*1.96)</f>
+      <c r="X3">
+        <f>(V3-W3)/(2*1.96)</f>
         <v>9.5747210595847784E-5</v>
       </c>
-      <c r="X3" s="1">
-        <f t="shared" ref="X3" si="9">(((1-T3)/(W3*W3))-(1/T3))*T3*T3</f>
+      <c r="Y3" s="1">
+        <f t="shared" ref="Y3" si="9">(((1-U3)/(X3*X3))-(1/U3))*U3*U3</f>
         <v>346.70270366901764</v>
       </c>
-      <c r="Y3" s="1">
-        <f t="shared" ref="Y3" si="10">X3*((1/T3)-1)</f>
+      <c r="Z3" s="1">
+        <f t="shared" ref="Z3" si="10">Y3*((1/U3)-1)</f>
         <v>193949.15471102181</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="K4" s="1"/>
-      <c r="N4" s="1"/>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="B4" s="4"/>
+      <c r="L4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
-      <c r="W4" s="1"/>
+      <c r="Q4" s="1"/>
       <c r="X4" s="1"/>
+      <c r="Y4" s="1"/>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="B5" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1287,7 +1357,7 @@
   <dimension ref="A1:Z3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1295,7 +1365,7 @@
     <col min="2" max="2" width="19.05078125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:26" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1375,7 +1445,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:26" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -1383,12 +1453,15 @@
         <v>27</v>
       </c>
       <c r="C2">
+        <f>VALUE(LEFT(B2, FIND("(", B2) - 1))</f>
         <v>0.03</v>
       </c>
       <c r="D2">
+        <f>VALUE(SUBSTITUTE(RIGHT(B2, LEN(B2) - FIND("(", B2)), _xlfn.CONCAT("-", SUBSTITUTE(RIGHT(B2, LEN(B2) - FIND("-", B2)), ")", ""), ")"), ""))</f>
         <v>0.01</v>
       </c>
       <c r="E2">
+        <f>VALUE(SUBSTITUTE(RIGHT(B2, LEN(B2) - FIND("-", B2)), ")", ""))</f>
         <v>0.09</v>
       </c>
       <c r="F2">
@@ -1476,20 +1549,23 @@
         <v>15326.332743796918</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:26" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A3" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>28</v>
       </c>
       <c r="C3">
+        <f>VALUE(LEFT(B3, FIND("(", B3) - 1))</f>
         <v>0.42</v>
       </c>
       <c r="D3">
+        <f>VALUE(SUBSTITUTE(RIGHT(B3, LEN(B3) - FIND("(", B3)), _xlfn.CONCAT("-", SUBSTITUTE(RIGHT(B3, LEN(B3) - FIND("-", B3)), ")", ""), ")"), ""))</f>
         <v>0.37</v>
       </c>
       <c r="E3">
+        <f>VALUE(SUBSTITUTE(RIGHT(B3, LEN(B3) - FIND("-", B3)), ")", ""))</f>
         <v>0.49</v>
       </c>
       <c r="F3">
@@ -1586,8 +1662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1595,7 +1671,7 @@
     <col min="2" max="2" width="19.47265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:26" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1675,7 +1751,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:26" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -1683,12 +1759,15 @@
         <v>29</v>
       </c>
       <c r="C2">
+        <f>VALUE(LEFT(B2, FIND("(", B2) - 1))</f>
         <v>0.02</v>
       </c>
       <c r="D2">
+        <f>VALUE(SUBSTITUTE(RIGHT(B2, LEN(B2) - FIND("(", B2)), _xlfn.CONCAT("-", SUBSTITUTE(RIGHT(B2, LEN(B2) - FIND("-", B2)), ")", ""), ")"), ""))</f>
         <v>0</v>
       </c>
       <c r="E2">
+        <f>VALUE(SUBSTITUTE(RIGHT(B2, LEN(B2) - FIND("-", B2)), ")", ""))</f>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="F2">
@@ -1776,20 +1855,23 @@
         <v>13344.93528854523</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:26" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A3" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C3">
+        <f>VALUE(LEFT(B3, FIND("(", B3) - 1))</f>
         <v>0.34</v>
       </c>
       <c r="D3">
-        <v>0.34</v>
+        <f>VALUE(SUBSTITUTE(RIGHT(B3, LEN(B3) - FIND("(", B3)), _xlfn.CONCAT("-", SUBSTITUTE(RIGHT(B3, LEN(B3) - FIND("-", B3)), ")", ""), ")"), ""))</f>
+        <v>0.28999999999999998</v>
       </c>
       <c r="E3">
+        <f>VALUE(SUBSTITUTE(RIGHT(B3, LEN(B3) - FIND("-", B3)), ")", ""))</f>
         <v>0.4</v>
       </c>
       <c r="F3">
@@ -1798,7 +1880,7 @@
       </c>
       <c r="G3">
         <f t="shared" si="0"/>
-        <v>3.4000000000000002E-4</v>
+        <v>2.9E-4</v>
       </c>
       <c r="H3">
         <f t="shared" si="0"/>
@@ -1814,7 +1896,7 @@
       </c>
       <c r="K3">
         <f>G3*3.28</f>
-        <v>1.1152E-3</v>
+        <v>9.5119999999999992E-4</v>
       </c>
       <c r="L3">
         <f>1-EXP(-I3)</f>
@@ -1826,19 +1908,19 @@
       </c>
       <c r="N3">
         <f t="shared" si="1"/>
-        <v>1.1145783955726074E-3</v>
+        <v>9.5074775268388922E-4</v>
       </c>
       <c r="O3">
         <f>(M3-N3)/(2*1.96)</f>
-        <v>5.0143190996043468E-5</v>
+        <v>9.1936722345206269E-5</v>
       </c>
       <c r="P3" s="1">
         <f t="shared" si="2"/>
-        <v>493.52822976454223</v>
+        <v>146.80998213754683</v>
       </c>
       <c r="Q3" s="1">
         <f t="shared" ref="Q3" si="6">P3*((1/L3)-1)</f>
-        <v>442300.11618767935</v>
+        <v>131571.14069832955</v>
       </c>
       <c r="R3">
         <f>F3*4.7</f>
@@ -1850,7 +1932,7 @@
       </c>
       <c r="T3">
         <f>G3*4.7</f>
-        <v>1.5980000000000002E-3</v>
+        <v>1.3630000000000001E-3</v>
       </c>
       <c r="U3">
         <f>1-EXP(-R3)</f>
@@ -1862,19 +1944,19 @@
       </c>
       <c r="W3">
         <f t="shared" si="3"/>
-        <v>1.5967238778382686E-3</v>
+        <v>1.362071537379439E-3</v>
       </c>
       <c r="X3">
         <f>(V3-W3)/(2*1.96)</f>
-        <v>7.1813782930285164E-5</v>
+        <v>1.3167407386366009E-4</v>
       </c>
       <c r="Y3" s="1">
         <f t="shared" si="4"/>
-        <v>493.56985031122116</v>
+        <v>146.81159907325244</v>
       </c>
       <c r="Z3" s="1">
         <f t="shared" si="5"/>
-        <v>308620.52129702154</v>
+        <v>91798.703283571289</v>
       </c>
     </row>
   </sheetData>

</xml_diff>